<commit_message>
Registro de tiempos e interfaces gráficas
Se agregaron las interfaces gráficas de los CU 5 y 8 y se hicieron algunos ajustes menores a otra interfaz
</commit_message>
<xml_diff>
--- a/Plantillas/Entrega 2/Planeación - Plantilla Lista de Tareas de la Entrega2 - copia.xlsx
+++ b/Plantillas/Entrega 2/Planeación - Plantilla Lista de Tareas de la Entrega2 - copia.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Dropbox\Proyecto Desarrollo de Software\plantillas\Iteración 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iro19\Documents\GitHub\Repositorio-Desarrollo-de-Software\Plantillas\Entrega 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E08D53-47C3-4132-8746-DD79E5ED99FD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B485AC-18C6-43E3-BC2D-E935FE4568EB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="105">
   <si>
     <t>Columna</t>
   </si>
@@ -347,6 +347,12 @@
   </si>
   <si>
     <t>Modelo de dominio (40%)</t>
+  </si>
+  <si>
+    <t>En este caso de uso el Maestro podrá registrar los pagos mensuales que realicen los alumnos de acuerdo a la clase correspondiente</t>
+  </si>
+  <si>
+    <t>CU-05</t>
   </si>
 </sst>
 </file>
@@ -532,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -619,12 +625,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -671,6 +671,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1020,10 +1029,10 @@
   <dimension ref="B1:BA100"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,84 +1107,84 @@
       </c>
     </row>
     <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="35"/>
+      <c r="I4" s="51"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="34" t="s">
+      <c r="K4" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="35"/>
+      <c r="L4" s="51"/>
       <c r="M4" s="8"/>
-      <c r="N4" s="34" t="s">
+      <c r="N4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="35"/>
+      <c r="O4" s="51"/>
       <c r="P4" s="8"/>
-      <c r="Q4" s="34" t="s">
+      <c r="Q4" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="35"/>
+      <c r="R4" s="51"/>
       <c r="S4" s="8"/>
-      <c r="T4" s="34" t="s">
+      <c r="T4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="35"/>
+      <c r="U4" s="51"/>
       <c r="V4" s="8"/>
-      <c r="W4" s="34" t="s">
+      <c r="W4" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="35"/>
+      <c r="X4" s="51"/>
       <c r="Y4" s="8"/>
-      <c r="Z4" s="34" t="s">
+      <c r="Z4" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="35"/>
+      <c r="AA4" s="51"/>
       <c r="AB4" s="8"/>
-      <c r="AC4" s="34" t="s">
+      <c r="AC4" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="35"/>
+      <c r="AD4" s="51"/>
       <c r="AE4" s="8"/>
-      <c r="AF4" s="34" t="s">
+      <c r="AF4" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="35"/>
+      <c r="AG4" s="51"/>
       <c r="AH4" s="8"/>
-      <c r="AI4" s="34" t="s">
+      <c r="AI4" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="35"/>
+      <c r="AJ4" s="51"/>
       <c r="AK4" s="8"/>
-      <c r="AL4" s="34" t="s">
+      <c r="AL4" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="35"/>
+      <c r="AM4" s="51"/>
       <c r="AN4" s="8"/>
-      <c r="AO4" s="34" t="s">
+      <c r="AO4" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="35"/>
+      <c r="AP4" s="51"/>
       <c r="AQ4" s="8"/>
-      <c r="AR4" s="34" t="s">
+      <c r="AR4" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="35"/>
+      <c r="AS4" s="51"/>
       <c r="AT4" s="8"/>
-      <c r="AU4" s="34" t="s">
+      <c r="AU4" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="35"/>
+      <c r="AV4" s="51"/>
       <c r="AW4" s="8"/>
-      <c r="AX4" s="34" t="s">
+      <c r="AX4" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="35"/>
-      <c r="AZ4" s="34" t="s">
+      <c r="AY4" s="51"/>
+      <c r="AZ4" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="35"/>
+      <c r="BA4" s="51"/>
     </row>
     <row r="5" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1366,7 +1375,7 @@
       <c r="BA6" s="17"/>
     </row>
     <row r="7" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="43"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="24"/>
       <c r="D7" s="19" t="s">
         <v>56</v>
@@ -1489,8 +1498,8 @@
       <c r="C8" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="22"/>
       <c r="G8" s="29"/>
       <c r="H8" s="15"/>
@@ -3064,9 +3073,9 @@
       <c r="C26" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" s="44"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
       <c r="G26" s="30"/>
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
@@ -3116,9 +3125,9 @@
       <c r="BA26" s="17"/>
     </row>
     <row r="27" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="43"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="46" t="s">
+      <c r="B27" s="41"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="44" t="s">
         <v>56</v>
       </c>
       <c r="E27" s="23" t="s">
@@ -3237,9 +3246,9 @@
       <c r="C28" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="29"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
@@ -3289,8 +3298,8 @@
       <c r="BA28" s="17"/>
     </row>
     <row r="29" spans="2:53" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="43"/>
-      <c r="C29" s="45"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="43"/>
       <c r="D29" s="19" t="s">
         <v>56</v>
       </c>
@@ -3412,9 +3421,9 @@
       <c r="C30" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="44"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
       <c r="G30" s="29"/>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
@@ -3464,7 +3473,7 @@
       <c r="BA30" s="17"/>
     </row>
     <row r="31" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B31" s="43"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="24"/>
       <c r="D31" s="19" t="s">
         <v>56</v>
@@ -3587,9 +3596,9 @@
       <c r="C32" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
       <c r="G32" s="29"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
@@ -3760,7 +3769,7 @@
       <c r="C34" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="44"/>
+      <c r="D34" s="42"/>
       <c r="E34" s="21"/>
       <c r="F34" s="12"/>
       <c r="G34" s="29"/>
@@ -3927,7 +3936,7 @@
       </c>
     </row>
     <row r="36" spans="2:53" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="43"/>
+      <c r="B36" s="41"/>
       <c r="C36" s="24" t="s">
         <v>74</v>
       </c>
@@ -4098,7 +4107,7 @@
       </c>
     </row>
     <row r="38" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B38" s="43"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="24" t="s">
         <v>77</v>
       </c>
@@ -4269,7 +4278,7 @@
       </c>
     </row>
     <row r="40" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B40" s="43"/>
+      <c r="B40" s="41"/>
       <c r="C40" s="24" t="s">
         <v>79</v>
       </c>
@@ -4672,10 +4681,10 @@
       <c r="D45" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="E45" s="44" t="s">
+      <c r="E45" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="F45" s="44" t="s">
+      <c r="F45" s="42" t="s">
         <v>81</v>
       </c>
       <c r="G45" s="29">
@@ -5014,10 +5023,10 @@
       <c r="D49" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="E49" s="44" t="s">
+      <c r="E49" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="F49" s="44" t="s">
+      <c r="F49" s="42" t="s">
         <v>81</v>
       </c>
       <c r="G49" s="29">
@@ -5353,7 +5362,7 @@
     <row r="53" spans="2:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="29"/>
       <c r="C53" s="19"/>
-      <c r="D53" s="47" t="s">
+      <c r="D53" s="45" t="s">
         <v>90</v>
       </c>
       <c r="E53" s="15" t="s">
@@ -5521,7 +5530,7 @@
     <row r="55" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B55" s="29"/>
       <c r="C55" s="19"/>
-      <c r="D55" s="47" t="s">
+      <c r="D55" s="45" t="s">
         <v>90</v>
       </c>
       <c r="E55" s="15" t="s">
@@ -5692,7 +5701,7 @@
     <row r="57" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B57" s="29"/>
       <c r="C57" s="19"/>
-      <c r="D57" s="47" t="s">
+      <c r="D57" s="45" t="s">
         <v>90</v>
       </c>
       <c r="E57" s="15" t="s">
@@ -5863,7 +5872,7 @@
     <row r="59" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B59" s="29"/>
       <c r="C59" s="12"/>
-      <c r="D59" s="47" t="s">
+      <c r="D59" s="45" t="s">
         <v>90</v>
       </c>
       <c r="E59" s="15" t="s">
@@ -6034,7 +6043,7 @@
     <row r="61" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B61" s="29"/>
       <c r="C61" s="12"/>
-      <c r="D61" s="47" t="s">
+      <c r="D61" s="45" t="s">
         <v>90</v>
       </c>
       <c r="E61" s="15" t="s">
@@ -6148,7 +6157,7 @@
       <c r="B62" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C62" s="42" t="s">
+      <c r="C62" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D62" s="19"/>
@@ -6205,7 +6214,7 @@
     <row r="63" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="29"/>
       <c r="C63" s="12"/>
-      <c r="D63" s="47" t="s">
+      <c r="D63" s="45" t="s">
         <v>90</v>
       </c>
       <c r="E63" s="15" t="s">
@@ -6322,10 +6331,10 @@
       <c r="C64" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="D64" s="48"/>
+      <c r="D64" s="46"/>
       <c r="E64" s="15"/>
       <c r="F64" s="15"/>
-      <c r="G64" s="49"/>
+      <c r="G64" s="47"/>
       <c r="H64" s="15"/>
       <c r="I64" s="15"/>
       <c r="J64" s="16"/>
@@ -6376,7 +6385,7 @@
     <row r="65" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B65" s="29"/>
       <c r="C65" s="19"/>
-      <c r="D65" s="47" t="s">
+      <c r="D65" s="45" t="s">
         <v>90</v>
       </c>
       <c r="E65" s="15" t="s">
@@ -6545,7 +6554,7 @@
       <c r="BA66" s="17"/>
     </row>
     <row r="67" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B67" s="50"/>
+      <c r="B67" s="48"/>
       <c r="C67" s="19"/>
       <c r="D67" s="22" t="s">
         <v>98</v>
@@ -6716,7 +6725,7 @@
       <c r="BA68" s="17"/>
     </row>
     <row r="69" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B69" s="50"/>
+      <c r="B69" s="48"/>
       <c r="C69" s="19"/>
       <c r="D69" s="22" t="s">
         <v>98</v>
@@ -6887,7 +6896,7 @@
       <c r="BA70" s="17"/>
     </row>
     <row r="71" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B71" s="50"/>
+      <c r="B71" s="48"/>
       <c r="C71" s="19"/>
       <c r="D71" s="22" t="s">
         <v>98</v>
@@ -6999,12 +7008,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="2:53" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="C72" s="12" t="s">
-        <v>57</v>
+        <v>104</v>
+      </c>
+      <c r="C72" s="52" t="s">
+        <v>103</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="5"/>
@@ -7058,7 +7067,7 @@
       <c r="BA72" s="17"/>
     </row>
     <row r="73" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B73" s="50"/>
+      <c r="B73" s="48"/>
       <c r="C73" s="19"/>
       <c r="D73" s="22" t="s">
         <v>98</v>
@@ -7229,7 +7238,7 @@
       <c r="BA74" s="17"/>
     </row>
     <row r="75" spans="2:53" ht="30" x14ac:dyDescent="0.25">
-      <c r="B75" s="50"/>
+      <c r="B75" s="48"/>
       <c r="C75" s="19"/>
       <c r="D75" s="22" t="s">
         <v>98</v>
@@ -7400,7 +7409,7 @@
       <c r="BA76" s="17"/>
     </row>
     <row r="77" spans="2:53" ht="30" x14ac:dyDescent="0.25">
-      <c r="B77" s="50"/>
+      <c r="B77" s="48"/>
       <c r="C77" s="19"/>
       <c r="D77" s="22" t="s">
         <v>98</v>
@@ -7569,7 +7578,7 @@
       <c r="BA78" s="17"/>
     </row>
     <row r="79" spans="2:53" ht="30" x14ac:dyDescent="0.25">
-      <c r="B79" s="50"/>
+      <c r="B79" s="48"/>
       <c r="C79" s="19"/>
       <c r="D79" s="22" t="s">
         <v>98</v>
@@ -7738,7 +7747,7 @@
       <c r="BA80" s="17"/>
     </row>
     <row r="81" spans="2:53" ht="30" x14ac:dyDescent="0.25">
-      <c r="B81" s="50"/>
+      <c r="B81" s="48"/>
       <c r="C81" s="19"/>
       <c r="D81" s="22" t="s">
         <v>98</v>
@@ -7907,7 +7916,7 @@
       <c r="BA82" s="17"/>
     </row>
     <row r="83" spans="2:53" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="50"/>
+      <c r="B83" s="48"/>
       <c r="C83" s="19"/>
       <c r="D83" s="22" t="s">
         <v>98</v>
@@ -8075,7 +8084,7 @@
       <c r="BA84" s="17"/>
     </row>
     <row r="85" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B85" s="50"/>
+      <c r="B85" s="48"/>
       <c r="C85" s="19"/>
       <c r="D85" s="22" t="s">
         <v>98</v>
@@ -8189,7 +8198,7 @@
       <c r="B86" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C86" s="42" t="s">
+      <c r="C86" s="40" t="s">
         <v>97</v>
       </c>
       <c r="D86" s="13"/>
@@ -8244,7 +8253,7 @@
       <c r="BA86" s="17"/>
     </row>
     <row r="87" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B87" s="50"/>
+      <c r="B87" s="48"/>
       <c r="C87" s="19"/>
       <c r="D87" s="22" t="s">
         <v>98</v>
@@ -8748,8 +8757,8 @@
     </row>
     <row r="93" spans="2:53" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="20"/>
-      <c r="C93" s="51"/>
-      <c r="D93" s="47" t="s">
+      <c r="C93" s="49"/>
+      <c r="D93" s="45" t="s">
         <v>102</v>
       </c>
       <c r="E93" s="15" t="s">
@@ -9335,60 +9344,65 @@
       </c>
     </row>
     <row r="100" spans="2:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C100" s="36"/>
-      <c r="D100" s="37"/>
-      <c r="E100" s="38"/>
+      <c r="C100" s="34"/>
+      <c r="D100" s="35"/>
+      <c r="E100" s="36"/>
       <c r="F100" s="25"/>
-      <c r="G100" s="39"/>
+      <c r="G100" s="37"/>
       <c r="H100" s="25"/>
       <c r="I100" s="25"/>
-      <c r="J100" s="40"/>
+      <c r="J100" s="38"/>
       <c r="K100" s="25"/>
       <c r="L100" s="25"/>
-      <c r="M100" s="40"/>
+      <c r="M100" s="38"/>
       <c r="N100" s="25"/>
       <c r="O100" s="25"/>
-      <c r="P100" s="40"/>
+      <c r="P100" s="38"/>
       <c r="Q100" s="25"/>
       <c r="R100" s="25"/>
-      <c r="S100" s="40"/>
+      <c r="S100" s="38"/>
       <c r="T100" s="25"/>
       <c r="U100" s="25"/>
-      <c r="V100" s="40"/>
+      <c r="V100" s="38"/>
       <c r="W100" s="25"/>
       <c r="X100" s="25"/>
-      <c r="Y100" s="40"/>
+      <c r="Y100" s="38"/>
       <c r="Z100" s="25"/>
       <c r="AA100" s="25"/>
-      <c r="AB100" s="40"/>
+      <c r="AB100" s="38"/>
       <c r="AC100" s="25"/>
       <c r="AD100" s="25"/>
-      <c r="AE100" s="40"/>
+      <c r="AE100" s="38"/>
       <c r="AF100" s="25"/>
       <c r="AG100" s="25"/>
-      <c r="AH100" s="40"/>
+      <c r="AH100" s="38"/>
       <c r="AI100" s="25"/>
       <c r="AJ100" s="25"/>
-      <c r="AK100" s="40"/>
+      <c r="AK100" s="38"/>
       <c r="AL100" s="25"/>
       <c r="AM100" s="25"/>
-      <c r="AN100" s="40"/>
+      <c r="AN100" s="38"/>
       <c r="AO100" s="25"/>
       <c r="AP100" s="25"/>
-      <c r="AQ100" s="40"/>
+      <c r="AQ100" s="38"/>
       <c r="AR100" s="25"/>
       <c r="AS100" s="25"/>
-      <c r="AT100" s="40"/>
+      <c r="AT100" s="38"/>
       <c r="AU100" s="25"/>
       <c r="AV100" s="25"/>
-      <c r="AW100" s="40"/>
+      <c r="AW100" s="38"/>
       <c r="AX100" s="25"/>
       <c r="AY100" s="25"/>
-      <c r="AZ100" s="41"/>
-      <c r="BA100" s="41"/>
+      <c r="AZ100" s="39"/>
+      <c r="BA100" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -9400,11 +9414,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="84" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>